<commit_message>
Updated code for NC routine and conditional cleaning.  Code for merging routine and conditional and writing into csv.
</commit_message>
<xml_diff>
--- a/data/nc/conditional_sampling_ncdmf/datasheets/cond_c1.xlsx
+++ b/data/nc/conditional_sampling_ncdmf/datasheets/cond_c1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahaines\Desktop\Method Comparison\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/megancarr/Documents/400_data_analytics/shellbase_with_usc/data/nc/conditional_sampling_ncdmf/datasheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98450645-B37B-C243-9EF0-6994313C1B22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7860" yWindow="75" windowWidth="14730" windowHeight="15285"/>
+    <workbookView xWindow="7860" yWindow="500" windowWidth="14740" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COND. FC" sheetId="1" r:id="rId1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>STATION</t>
   </si>
@@ -60,12 +61,6 @@
   </si>
   <si>
     <t>Fullard Creek is #6 in both runs</t>
-  </si>
-  <si>
-    <t>2/3 EBB</t>
-  </si>
-  <si>
-    <t>C</t>
   </si>
   <si>
     <t>CM #17</t>
@@ -107,7 +102,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
@@ -292,6 +287,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -327,6 +339,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -502,47 +531,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr transitionEvaluation="1"/>
   <dimension ref="A1:MP39"/>
   <sheetViews>
     <sheetView tabSelected="1" defaultGridColor="0" colorId="22" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="MM1" activePane="topRight" state="frozenSplit"/>
-      <selection pane="topRight" activeCell="MP1" sqref="MP1:MP1048576"/>
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.7109375" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" style="10"/>
-    <col min="2" max="2" width="10.88671875" style="13" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="191" width="7.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="192" max="192" width="11.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="193" max="193" width="20.21875" style="8" bestFit="1" customWidth="1"/>
-    <col min="194" max="259" width="7.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="260" max="260" width="7.44140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="261" max="261" width="9.21875" style="10" bestFit="1" customWidth="1"/>
-    <col min="262" max="262" width="7.44140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="263" max="264" width="7.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="265" max="267" width="7.44140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="268" max="293" width="7.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="294" max="294" width="7.44140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="295" max="297" width="11.77734375" style="10"/>
-    <col min="298" max="298" width="11.77734375" style="8"/>
-    <col min="299" max="314" width="7.44140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="315" max="315" width="7.44140625" style="10" customWidth="1"/>
-    <col min="316" max="316" width="11.77734375" style="10"/>
-    <col min="317" max="317" width="7.44140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="318" max="328" width="11.77734375" style="10"/>
-    <col min="329" max="329" width="11.77734375" style="17"/>
-    <col min="330" max="354" width="11.77734375" style="10"/>
-    <col min="355" max="16384" width="11.77734375" style="8"/>
+    <col min="1" max="1" width="11.7109375" style="10"/>
+    <col min="2" max="2" width="10.85546875" style="13" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="191" width="7.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="192" max="192" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="193" max="193" width="20.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="194" max="259" width="7.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="260" max="260" width="7.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="261" max="261" width="9.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="262" max="262" width="7.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="263" max="264" width="7.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="265" max="267" width="7.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="268" max="293" width="7.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="294" max="294" width="7.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="295" max="297" width="11.7109375" style="10"/>
+    <col min="298" max="298" width="11.7109375" style="8"/>
+    <col min="299" max="314" width="7.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="315" max="315" width="7.42578125" style="10" customWidth="1"/>
+    <col min="316" max="316" width="11.7109375" style="10"/>
+    <col min="317" max="317" width="7.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="318" max="328" width="11.7109375" style="10"/>
+    <col min="329" max="329" width="11.7109375" style="17"/>
+    <col min="330" max="354" width="11.7109375" style="10"/>
+    <col min="355" max="16384" width="11.7109375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:354" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:354" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1115,7 +1144,7 @@
         <v>39493</v>
       </c>
       <c r="GJ1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="GK1" s="1">
         <v>39582</v>
@@ -1604,9 +1633,9 @@
         <v>44231</v>
       </c>
     </row>
-    <row r="2" spans="1:354" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:354" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2" s="9">
         <v>16</v>
@@ -2454,7 +2483,7 @@
         <v>22</v>
       </c>
       <c r="KL2" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="KM2" s="10">
         <v>4</v>
@@ -2616,15 +2645,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:354" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:354" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" s="9">
         <v>12</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -3049,9 +3078,9 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="4" spans="1:354" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:354" x14ac:dyDescent="0.15">
       <c r="A4" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" s="9">
         <v>8</v>
@@ -3420,9 +3449,9 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="5" spans="1:354" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:354" x14ac:dyDescent="0.15">
       <c r="A5" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" s="9">
         <v>6</v>
@@ -3862,9 +3891,9 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="6" spans="1:354" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:354" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" s="9">
         <v>7</v>
@@ -3981,7 +4010,7 @@
         <v>7.8</v>
       </c>
       <c r="KL6" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="KM6" s="10">
         <v>17</v>
@@ -4122,7 +4151,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="7" spans="1:354" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:354" ht="28" x14ac:dyDescent="0.15">
       <c r="A7" s="4"/>
       <c r="B7" s="5">
         <v>40</v>
@@ -4318,7 +4347,7 @@
       <c r="GI7" s="4"/>
       <c r="GJ7" s="4"/>
       <c r="GK7" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="GL7" s="4">
         <v>1.7</v>
@@ -4565,7 +4594,7 @@
       <c r="LF7" s="4"/>
       <c r="LG7" s="4"/>
     </row>
-    <row r="8" spans="1:354" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:354" ht="14" x14ac:dyDescent="0.15">
       <c r="B8" s="9">
         <v>11</v>
       </c>
@@ -5170,7 +5199,7 @@
         <v>4</v>
       </c>
       <c r="JA8" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="JB8" s="11">
         <v>13</v>
@@ -5275,7 +5304,7 @@
         <v>6.8</v>
       </c>
       <c r="KL8" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="KM8" s="10">
         <v>2</v>
@@ -5326,7 +5355,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="9" spans="1:354" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:354" x14ac:dyDescent="0.15">
       <c r="B9" s="9">
         <v>8</v>
       </c>
@@ -5556,7 +5585,7 @@
       <c r="FV9" s="1"/>
       <c r="KP9" s="11"/>
     </row>
-    <row r="10" spans="1:354" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:354" x14ac:dyDescent="0.15">
       <c r="B10" s="9">
         <v>11</v>
       </c>
@@ -5848,7 +5877,7 @@
       <c r="FR10" s="11"/>
       <c r="FS10" s="11"/>
     </row>
-    <row r="11" spans="1:354" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:354" x14ac:dyDescent="0.15">
       <c r="B11" s="9">
         <v>20</v>
       </c>
@@ -6047,7 +6076,7 @@
       <c r="FR11" s="11"/>
       <c r="FS11" s="11"/>
     </row>
-    <row r="12" spans="1:354" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:354" x14ac:dyDescent="0.15">
       <c r="B12" s="13" t="s">
         <v>3</v>
       </c>
@@ -6226,7 +6255,7 @@
       <c r="FR12" s="11"/>
       <c r="FS12" s="11"/>
     </row>
-    <row r="13" spans="1:354" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:354" x14ac:dyDescent="0.15">
       <c r="B13" s="9" t="s">
         <v>4</v>
       </c>
@@ -6407,7 +6436,7 @@
       <c r="FR13" s="11"/>
       <c r="FS13" s="11"/>
     </row>
-    <row r="14" spans="1:354" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:354" x14ac:dyDescent="0.15">
       <c r="B14" s="13" t="s">
         <v>5</v>
       </c>
@@ -6589,7 +6618,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="15" spans="1:354" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:354" x14ac:dyDescent="0.15">
       <c r="B15" s="13" t="s">
         <v>6</v>
       </c>
@@ -6766,7 +6795,7 @@
       <c r="FR15" s="11"/>
       <c r="FS15" s="11"/>
     </row>
-    <row r="16" spans="1:354" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:354" x14ac:dyDescent="0.15">
       <c r="B16" s="13" t="s">
         <v>7</v>
       </c>
@@ -6946,7 +6975,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:317" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:317" x14ac:dyDescent="0.15">
       <c r="B17" s="13" t="s">
         <v>8</v>
       </c>
@@ -7126,7 +7155,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="18" spans="2:317" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:317" x14ac:dyDescent="0.15">
       <c r="B18" s="9">
         <v>3</v>
       </c>
@@ -7305,7 +7334,7 @@
       <c r="FR18" s="11"/>
       <c r="FS18" s="11"/>
     </row>
-    <row r="19" spans="2:317" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:317" x14ac:dyDescent="0.15">
       <c r="B19" s="9">
         <v>1</v>
       </c>
@@ -7313,426 +7342,71 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:317" x14ac:dyDescent="0.2">
-      <c r="D20" s="14">
-        <v>35684</v>
-      </c>
-      <c r="E20" s="8">
-        <v>2</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H20" s="8">
-        <v>35</v>
-      </c>
-      <c r="I20" s="8">
-        <v>17</v>
-      </c>
-      <c r="J20" s="8">
-        <v>1.2303999999999999</v>
-      </c>
+    <row r="20" spans="2:317" x14ac:dyDescent="0.15">
+      <c r="D20" s="14"/>
     </row>
-    <row r="21" spans="2:317" x14ac:dyDescent="0.2">
-      <c r="D21" s="14">
-        <v>35684</v>
-      </c>
-      <c r="E21" s="8">
-        <v>21</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H21" s="8">
-        <v>36</v>
-      </c>
-      <c r="I21" s="8">
-        <v>7.8</v>
-      </c>
-      <c r="J21" s="8">
-        <v>0.8921</v>
-      </c>
+    <row r="21" spans="2:317" x14ac:dyDescent="0.15">
+      <c r="D21" s="14"/>
       <c r="GJ21" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="22" spans="2:317" x14ac:dyDescent="0.2">
-      <c r="D22" s="14">
-        <v>35684</v>
-      </c>
-      <c r="E22" s="8">
-        <v>23</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H22" s="8">
-        <v>37</v>
-      </c>
-      <c r="I22" s="8">
-        <v>130</v>
-      </c>
-      <c r="J22" s="8">
-        <v>2.1139000000000001</v>
-      </c>
+    <row r="22" spans="2:317" x14ac:dyDescent="0.15">
+      <c r="D22" s="14"/>
     </row>
-    <row r="23" spans="2:317" x14ac:dyDescent="0.2">
-      <c r="D23" s="14">
-        <v>35684</v>
-      </c>
-      <c r="E23" s="8">
-        <v>1</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H23" s="8">
-        <v>35</v>
-      </c>
-      <c r="I23" s="8">
-        <v>350</v>
-      </c>
-      <c r="J23" s="8">
-        <v>2.5440999999999998</v>
-      </c>
+    <row r="23" spans="2:317" x14ac:dyDescent="0.15">
+      <c r="D23" s="14"/>
     </row>
-    <row r="24" spans="2:317" x14ac:dyDescent="0.2">
-      <c r="D24" s="14">
-        <v>35684</v>
-      </c>
-      <c r="E24" s="8">
-        <v>2</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H24" s="8">
-        <v>35</v>
-      </c>
-      <c r="I24" s="8">
-        <v>46</v>
-      </c>
-      <c r="J24" s="8">
-        <v>1.6628000000000001</v>
-      </c>
+    <row r="24" spans="2:317" x14ac:dyDescent="0.15">
+      <c r="D24" s="14"/>
     </row>
-    <row r="25" spans="2:317" x14ac:dyDescent="0.2">
-      <c r="D25" s="14">
-        <v>35684</v>
-      </c>
-      <c r="E25" s="8">
-        <v>3</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H25" s="8">
-        <v>35</v>
-      </c>
-      <c r="I25" s="8">
-        <v>23</v>
-      </c>
-      <c r="J25" s="8">
-        <v>1.3616999999999999</v>
-      </c>
+    <row r="25" spans="2:317" x14ac:dyDescent="0.15">
+      <c r="D25" s="14"/>
     </row>
-    <row r="26" spans="2:317" x14ac:dyDescent="0.2">
-      <c r="D26" s="14">
-        <v>35684</v>
-      </c>
-      <c r="E26" s="8">
-        <v>5</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H26" s="8">
-        <v>36</v>
-      </c>
-      <c r="I26" s="8">
-        <v>13</v>
-      </c>
-      <c r="J26" s="8">
-        <v>1.1138999999999999</v>
-      </c>
+    <row r="26" spans="2:317" x14ac:dyDescent="0.15">
+      <c r="D26" s="14"/>
     </row>
-    <row r="27" spans="2:317" x14ac:dyDescent="0.2">
-      <c r="D27" s="14">
-        <v>35684</v>
-      </c>
-      <c r="E27" s="8">
-        <v>6</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H27" s="8">
-        <v>35</v>
-      </c>
-      <c r="I27" s="8">
-        <v>23</v>
-      </c>
-      <c r="J27" s="8">
-        <v>1.3616999999999999</v>
-      </c>
+    <row r="27" spans="2:317" x14ac:dyDescent="0.15">
+      <c r="D27" s="14"/>
     </row>
-    <row r="28" spans="2:317" x14ac:dyDescent="0.2">
-      <c r="D28" s="14">
-        <v>35684</v>
-      </c>
-      <c r="E28" s="8">
-        <v>7</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H28" s="8">
-        <v>37</v>
-      </c>
-      <c r="I28" s="8">
-        <v>2</v>
-      </c>
-      <c r="J28" s="8">
-        <v>0.30099999999999999</v>
-      </c>
+    <row r="28" spans="2:317" x14ac:dyDescent="0.15">
+      <c r="D28" s="14"/>
     </row>
-    <row r="29" spans="2:317" x14ac:dyDescent="0.2">
-      <c r="D29" s="14">
-        <v>35684</v>
-      </c>
-      <c r="E29" s="8">
-        <v>8</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H29" s="8">
-        <v>36</v>
-      </c>
-      <c r="I29" s="8">
-        <v>6.8</v>
-      </c>
-      <c r="J29" s="8">
-        <v>0.83250000000000002</v>
-      </c>
+    <row r="29" spans="2:317" x14ac:dyDescent="0.15">
+      <c r="D29" s="14"/>
     </row>
-    <row r="30" spans="2:317" x14ac:dyDescent="0.2">
-      <c r="D30" s="14">
-        <v>35684</v>
-      </c>
-      <c r="E30" s="8">
-        <v>9</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H30" s="8">
-        <v>39</v>
-      </c>
-      <c r="I30" s="8">
-        <v>21</v>
-      </c>
-      <c r="J30" s="8">
-        <v>1.3222</v>
-      </c>
+    <row r="30" spans="2:317" x14ac:dyDescent="0.15">
+      <c r="D30" s="14"/>
     </row>
-    <row r="31" spans="2:317" x14ac:dyDescent="0.2">
-      <c r="D31" s="14">
-        <v>35684</v>
-      </c>
-      <c r="E31" s="8">
-        <v>10</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H31" s="8">
-        <v>38</v>
-      </c>
-      <c r="I31" s="8">
-        <v>4.5</v>
-      </c>
-      <c r="J31" s="8">
-        <v>0.6532</v>
-      </c>
+    <row r="31" spans="2:317" x14ac:dyDescent="0.15">
+      <c r="D31" s="14"/>
     </row>
-    <row r="32" spans="2:317" x14ac:dyDescent="0.2">
-      <c r="D32" s="14">
-        <v>35684</v>
-      </c>
-      <c r="E32" s="8">
-        <v>11</v>
-      </c>
-      <c r="G32" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H32" s="8">
-        <v>39</v>
-      </c>
-      <c r="I32" s="8">
-        <v>6.8</v>
-      </c>
-      <c r="J32" s="8">
-        <v>0.83250000000000002</v>
-      </c>
+    <row r="32" spans="2:317" x14ac:dyDescent="0.15">
+      <c r="D32" s="14"/>
     </row>
-    <row r="33" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D33" s="14">
-        <v>35684</v>
-      </c>
-      <c r="E33" s="8">
-        <v>12</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H33" s="8">
-        <v>39</v>
-      </c>
-      <c r="I33" s="8">
-        <v>1.7</v>
-      </c>
-      <c r="J33" s="8">
-        <v>0.23039999999999999</v>
-      </c>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D33" s="14"/>
     </row>
-    <row r="34" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D34" s="14">
-        <v>35684</v>
-      </c>
-      <c r="E34" s="8">
-        <v>13</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H34" s="8">
-        <v>39</v>
-      </c>
-      <c r="I34" s="8">
-        <v>1.7</v>
-      </c>
-      <c r="J34" s="8">
-        <v>0.23039999999999999</v>
-      </c>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D34" s="14"/>
     </row>
-    <row r="35" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D35" s="14">
-        <v>35684</v>
-      </c>
-      <c r="E35" s="8">
-        <v>16</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H35" s="8">
-        <v>39</v>
-      </c>
-      <c r="I35" s="8">
-        <v>2</v>
-      </c>
-      <c r="J35" s="8">
-        <v>0.30099999999999999</v>
-      </c>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D35" s="14"/>
     </row>
-    <row r="36" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D36" s="14">
-        <v>35684</v>
-      </c>
-      <c r="E36" s="8">
-        <v>17</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H36" s="8">
-        <v>36</v>
-      </c>
-      <c r="I36" s="8">
-        <v>70</v>
-      </c>
-      <c r="J36" s="8">
-        <v>1.8451</v>
-      </c>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D36" s="14"/>
     </row>
-    <row r="37" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D37" s="14">
-        <v>35684</v>
-      </c>
-      <c r="E37" s="8">
-        <v>20</v>
-      </c>
-      <c r="G37" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H37" s="8">
-        <v>39</v>
-      </c>
-      <c r="I37" s="8">
-        <v>14</v>
-      </c>
-      <c r="J37" s="8">
-        <v>1.1460999999999999</v>
-      </c>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D37" s="14"/>
     </row>
-    <row r="38" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D38" s="14">
-        <v>35684</v>
-      </c>
-      <c r="E38" s="8">
-        <v>21</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="G38" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H38" s="8">
-        <v>36</v>
-      </c>
-      <c r="I38" s="8">
-        <v>46</v>
-      </c>
-      <c r="J38" s="8">
-        <v>1.6628000000000001</v>
-      </c>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D38" s="14"/>
     </row>
-    <row r="39" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D39" s="14">
-        <v>35684</v>
-      </c>
-      <c r="E39" s="8">
-        <v>23</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="G39" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H39" s="8">
-        <v>37</v>
-      </c>
-      <c r="I39" s="8">
-        <v>17</v>
-      </c>
-      <c r="J39" s="8">
-        <v>1.2303999999999999</v>
-      </c>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D39" s="14"/>
     </row>
   </sheetData>
-  <sortState ref="A2:LG39">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:LG39">
     <sortCondition ref="A3:A39"/>
   </sortState>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>